<commit_message>
database : add deficiency files
</commit_message>
<xml_diff>
--- a/database/industries/dode/shekarbon/cost/quarterly.xlsx
+++ b/database/industries/dode/shekarbon/cost/quarterly.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\dode\shekarbon\cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\dode\shekarbon\cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408654F2-3C35-4AA1-98EF-252C627A6520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="5550"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="84">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -136,6 +137,42 @@
   </si>
   <si>
     <t>مقدار موجودی پایان دوره</t>
+  </si>
+  <si>
+    <t>مبلغ موجودی اول دوره</t>
+  </si>
+  <si>
+    <t>میلیون ریال</t>
+  </si>
+  <si>
+    <t>مبلغ خرید طی دوره</t>
+  </si>
+  <si>
+    <t>مبلغ مصرف طی دوره</t>
+  </si>
+  <si>
+    <t>مبلغ موجودی پایان دوره</t>
+  </si>
+  <si>
+    <t>نرخ موجودی اول دوره</t>
+  </si>
+  <si>
+    <t>عدد / ریال</t>
+  </si>
+  <si>
+    <t>تن / ریال</t>
+  </si>
+  <si>
+    <t>/ ریال</t>
+  </si>
+  <si>
+    <t>نرخ خرید طی دوره</t>
+  </si>
+  <si>
+    <t>نرخ مصرف طی دوره</t>
+  </si>
+  <si>
+    <t>نرخ موجودی پایان دوره</t>
   </si>
   <si>
     <t>هزینه سربار</t>
@@ -241,7 +278,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,7 +448,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -423,7 +460,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -470,6 +507,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -505,6 +559,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -656,17 +727,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:N172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -681,7 +752,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -698,7 +769,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -715,7 +786,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -730,7 +801,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="2:14" ht="42" x14ac:dyDescent="0.65">
+    <row r="5" spans="2:14" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -747,7 +818,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="2:14" ht="42" x14ac:dyDescent="0.65">
+    <row r="6" spans="2:14" ht="40.799999999999997" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -764,7 +835,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -779,7 +850,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
@@ -816,7 +887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -831,7 +902,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
@@ -868,7 +939,7 @@
         <v>3144092</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
@@ -905,7 +976,7 @@
         <v>40087</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>16</v>
       </c>
@@ -942,7 +1013,7 @@
         <v>295818</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
@@ -979,7 +1050,7 @@
         <v>3479997</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>19</v>
       </c>
@@ -1053,7 +1124,7 @@
         <v>3479997</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1090,7 +1161,7 @@
         <v>-88400</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>21</v>
       </c>
@@ -1127,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>22</v>
       </c>
@@ -1164,7 +1235,7 @@
         <v>3391597</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
@@ -1201,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
@@ -1238,7 +1309,7 @@
         <v>-205813</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
         <v>25</v>
       </c>
@@ -1275,7 +1346,7 @@
         <v>3185784</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
@@ -1312,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>27</v>
       </c>
@@ -1349,7 +1420,7 @@
         <v>3185784</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1364,7 +1435,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1379,7 +1450,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1394,7 +1465,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
         <v>28</v>
       </c>
@@ -1431,7 +1502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1446,7 +1517,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>29</v>
       </c>
@@ -1485,7 +1556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>32</v>
       </c>
@@ -1524,7 +1595,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
         <v>34</v>
       </c>
@@ -1563,7 +1634,7 @@
         <v>4953</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>35</v>
       </c>
@@ -1600,7 +1671,7 @@
         <v>179045</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +1708,7 @@
         <v>183998</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1652,7 +1723,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1667,7 +1738,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1682,7 +1753,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>36</v>
       </c>
@@ -1719,7 +1790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1734,7 +1805,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
         <v>29</v>
       </c>
@@ -1773,7 +1844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>32</v>
       </c>
@@ -1812,7 +1883,7 @@
         <v>8160</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
         <v>34</v>
       </c>
@@ -1851,7 +1922,7 @@
         <v>12115</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
         <v>35</v>
       </c>
@@ -1888,7 +1959,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="14" t="s">
         <v>17</v>
       </c>
@@ -1925,7 +1996,7 @@
         <v>110275</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1940,7 +2011,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1955,7 +2026,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1970,7 +2041,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B47" s="7" t="s">
         <v>37</v>
       </c>
@@ -2007,7 +2078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2022,7 +2093,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="s">
         <v>29</v>
       </c>
@@ -2061,7 +2132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B50" s="10" t="s">
         <v>32</v>
       </c>
@@ -2100,7 +2171,7 @@
         <v>8160</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
         <v>34</v>
       </c>
@@ -2139,7 +2210,7 @@
         <v>12041</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>35</v>
       </c>
@@ -2176,7 +2247,7 @@
         <v>153450</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>17</v>
       </c>
@@ -2213,7 +2284,7 @@
         <v>173651</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2228,7 +2299,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -2243,7 +2314,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -2258,7 +2329,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
         <v>38</v>
       </c>
@@ -2295,7 +2366,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -2310,7 +2381,7 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B59" s="8" t="s">
         <v>29</v>
       </c>
@@ -2349,7 +2420,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>32</v>
       </c>
@@ -2388,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B61" s="8" t="s">
         <v>34</v>
       </c>
@@ -2427,7 +2498,7 @@
         <v>5027</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
         <v>35</v>
       </c>
@@ -2464,7 +2535,7 @@
         <v>115595</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B63" s="14" t="s">
         <v>17</v>
       </c>
@@ -2501,7 +2572,7 @@
         <v>120622</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2516,7 +2587,7 @@
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -2531,7 +2602,7 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -2546,7 +2617,7 @@
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
     </row>
-    <row r="67" spans="2:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B67" s="7" t="s">
         <v>39</v>
       </c>
@@ -2583,7 +2654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2598,476 +2669,490 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B69" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C69" s="9"/>
       <c r="D69" s="9"/>
-      <c r="E69" s="9">
-        <v>0</v>
-      </c>
-      <c r="F69" s="9">
-        <v>0</v>
-      </c>
-      <c r="G69" s="9">
-        <v>7791</v>
-      </c>
-      <c r="H69" s="9">
-        <v>-7791</v>
-      </c>
-      <c r="I69" s="9">
-        <v>7681</v>
-      </c>
-      <c r="J69" s="9">
-        <v>-7681</v>
-      </c>
-      <c r="K69" s="9">
-        <v>0</v>
-      </c>
-      <c r="L69" s="9">
-        <v>0</v>
-      </c>
-      <c r="M69" s="9">
-        <v>0</v>
-      </c>
-      <c r="N69" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M69" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N69" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B70" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C70" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11">
-        <v>0</v>
+        <v>73836</v>
       </c>
       <c r="F70" s="11">
-        <v>0</v>
+        <v>24344</v>
       </c>
       <c r="G70" s="11">
-        <v>0</v>
+        <v>31827</v>
       </c>
       <c r="H70" s="11">
-        <v>0</v>
+        <v>44986</v>
       </c>
       <c r="I70" s="11">
-        <v>0</v>
+        <v>48120</v>
       </c>
       <c r="J70" s="11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="K70" s="11">
         <v>0</v>
       </c>
-      <c r="L70" s="11">
-        <v>0</v>
-      </c>
-      <c r="M70" s="11">
-        <v>0</v>
-      </c>
-      <c r="N70" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L70" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M70" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N70" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B71" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C71" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9">
-        <v>0</v>
+        <v>150789</v>
       </c>
       <c r="F71" s="9">
-        <v>0</v>
+        <v>63078</v>
       </c>
       <c r="G71" s="9">
-        <v>0</v>
+        <v>286295</v>
       </c>
       <c r="H71" s="9">
-        <v>0</v>
+        <v>305901</v>
       </c>
       <c r="I71" s="9">
-        <v>0</v>
+        <v>481226</v>
       </c>
       <c r="J71" s="9">
-        <v>0</v>
+        <v>503801</v>
       </c>
       <c r="K71" s="9">
-        <v>0</v>
-      </c>
-      <c r="L71" s="9">
-        <v>0</v>
+        <v>437758</v>
+      </c>
+      <c r="L71" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="M71" s="9">
-        <v>0</v>
+        <v>620819</v>
       </c>
       <c r="N71" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+        <v>783513</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B72" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C72" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11">
-        <v>0</v>
-      </c>
-      <c r="F72" s="11">
-        <v>0</v>
-      </c>
-      <c r="G72" s="11">
-        <v>0</v>
+        <v>35568</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="H72" s="11">
         <v>0</v>
       </c>
       <c r="I72" s="11">
-        <v>1</v>
+        <v>30918</v>
       </c>
       <c r="J72" s="11">
-        <v>-1</v>
+        <v>57685</v>
       </c>
       <c r="K72" s="11">
-        <v>0</v>
-      </c>
-      <c r="L72" s="11">
-        <v>0</v>
+        <v>68443</v>
+      </c>
+      <c r="L72" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="M72" s="11">
-        <v>0</v>
+        <v>95917</v>
       </c>
       <c r="N72" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9">
-        <v>13421</v>
-      </c>
-      <c r="F73" s="9">
-        <v>12999</v>
-      </c>
-      <c r="G73" s="9">
-        <v>27928</v>
-      </c>
-      <c r="H73" s="9">
-        <v>25727</v>
-      </c>
-      <c r="I73" s="9">
-        <v>27158</v>
-      </c>
-      <c r="J73" s="9">
-        <v>5915</v>
-      </c>
-      <c r="K73" s="9">
-        <v>11925</v>
-      </c>
-      <c r="L73" s="9">
-        <v>36397</v>
-      </c>
-      <c r="M73" s="9">
-        <v>21411</v>
-      </c>
-      <c r="N73" s="9">
-        <v>78269</v>
-      </c>
-    </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11">
-        <v>14291</v>
-      </c>
-      <c r="F74" s="11">
-        <v>16482</v>
-      </c>
-      <c r="G74" s="11">
-        <v>-2113</v>
-      </c>
-      <c r="H74" s="11">
-        <v>34349</v>
-      </c>
-      <c r="I74" s="11">
-        <v>73</v>
-      </c>
-      <c r="J74" s="11">
-        <v>56668</v>
-      </c>
-      <c r="K74" s="11">
-        <v>42850</v>
-      </c>
-      <c r="L74" s="11">
-        <v>85798</v>
-      </c>
-      <c r="M74" s="11">
-        <v>55878</v>
-      </c>
-      <c r="N74" s="11">
-        <v>50698</v>
-      </c>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9">
-        <v>6000</v>
-      </c>
-      <c r="F75" s="9">
-        <v>14166</v>
-      </c>
-      <c r="G75" s="9">
-        <v>-1</v>
-      </c>
-      <c r="H75" s="9">
-        <v>19271</v>
-      </c>
-      <c r="I75" s="9">
-        <v>4120</v>
-      </c>
-      <c r="J75" s="9">
-        <v>21417</v>
-      </c>
-      <c r="K75" s="9">
-        <v>16144</v>
-      </c>
-      <c r="L75" s="9">
-        <v>16807</v>
-      </c>
-      <c r="M75" s="9">
-        <v>19627</v>
-      </c>
-      <c r="N75" s="9">
-        <v>28194</v>
-      </c>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11">
-        <v>23704</v>
-      </c>
-      <c r="F76" s="11">
-        <v>54353</v>
-      </c>
-      <c r="G76" s="11">
-        <v>25152</v>
-      </c>
-      <c r="H76" s="11">
-        <v>66517</v>
-      </c>
-      <c r="I76" s="11">
-        <v>66200</v>
-      </c>
-      <c r="J76" s="11">
-        <v>57717</v>
-      </c>
-      <c r="K76" s="11">
-        <v>63151</v>
-      </c>
-      <c r="L76" s="11">
-        <v>71398</v>
-      </c>
-      <c r="M76" s="11">
-        <v>89715</v>
-      </c>
-      <c r="N76" s="11">
-        <v>112042</v>
-      </c>
-    </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9">
-        <v>0</v>
-      </c>
-      <c r="F77" s="9">
-        <v>0</v>
-      </c>
-      <c r="G77" s="9">
-        <v>0</v>
-      </c>
-      <c r="H77" s="9">
-        <v>0</v>
-      </c>
-      <c r="I77" s="9">
-        <v>0</v>
-      </c>
-      <c r="J77" s="9">
-        <v>0</v>
-      </c>
-      <c r="K77" s="9">
-        <v>0</v>
-      </c>
-      <c r="L77" s="9">
-        <v>0</v>
-      </c>
-      <c r="M77" s="9">
-        <v>0</v>
-      </c>
-      <c r="N77" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B78" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11">
-        <v>11124</v>
-      </c>
-      <c r="F78" s="11">
-        <v>63807</v>
-      </c>
-      <c r="G78" s="11">
-        <v>111345</v>
-      </c>
-      <c r="H78" s="11">
-        <v>4699</v>
-      </c>
-      <c r="I78" s="11">
-        <v>76241</v>
-      </c>
-      <c r="J78" s="11">
-        <v>22262</v>
-      </c>
-      <c r="K78" s="11">
-        <v>62862</v>
-      </c>
-      <c r="L78" s="11">
-        <v>85373</v>
-      </c>
-      <c r="M78" s="11">
-        <v>40060</v>
-      </c>
-      <c r="N78" s="11">
-        <v>26615</v>
-      </c>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B79" s="14" t="s">
+        <v>66284</v>
+      </c>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B73" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15">
-        <v>68540</v>
-      </c>
-      <c r="F79" s="15">
-        <v>161807</v>
-      </c>
-      <c r="G79" s="15">
-        <v>170102</v>
-      </c>
-      <c r="H79" s="15">
-        <v>142772</v>
-      </c>
-      <c r="I79" s="15">
-        <v>181474</v>
-      </c>
-      <c r="J79" s="15">
-        <v>156297</v>
-      </c>
-      <c r="K79" s="15">
-        <v>196932</v>
-      </c>
-      <c r="L79" s="15">
-        <v>295773</v>
-      </c>
-      <c r="M79" s="15">
-        <v>226691</v>
-      </c>
-      <c r="N79" s="15">
-        <v>295818</v>
-      </c>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
-    </row>
-    <row r="83" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B83" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
-    </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15">
+        <v>260193</v>
+      </c>
+      <c r="F73" s="15">
+        <v>87422</v>
+      </c>
+      <c r="G73" s="15">
+        <v>318122</v>
+      </c>
+      <c r="H73" s="15">
+        <v>350887</v>
+      </c>
+      <c r="I73" s="15">
+        <v>560264</v>
+      </c>
+      <c r="J73" s="15">
+        <v>561485</v>
+      </c>
+      <c r="K73" s="15">
+        <v>506201</v>
+      </c>
+      <c r="L73" s="15">
+        <v>0</v>
+      </c>
+      <c r="M73" s="15">
+        <v>716736</v>
+      </c>
+      <c r="N73" s="15">
+        <v>849797</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+    </row>
+    <row r="77" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B77" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L77" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B79" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F79" s="9">
+        <v>15862</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L79" s="9">
+        <v>218638</v>
+      </c>
+      <c r="M79" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N79" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B80" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11">
+        <v>42126</v>
+      </c>
+      <c r="F80" s="11">
+        <v>128808</v>
+      </c>
+      <c r="G80" s="11">
+        <v>120438</v>
+      </c>
+      <c r="H80" s="11">
+        <v>174528</v>
+      </c>
+      <c r="I80" s="11">
+        <v>13268</v>
+      </c>
+      <c r="J80" s="11">
+        <v>31101</v>
+      </c>
+      <c r="K80" s="11">
+        <v>172258</v>
+      </c>
+      <c r="L80" s="11">
+        <v>435780</v>
+      </c>
+      <c r="M80" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N80" s="11">
+        <v>1247385</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B81" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9">
+        <v>260290</v>
+      </c>
+      <c r="F81" s="9">
+        <v>708011</v>
+      </c>
+      <c r="G81" s="9">
+        <v>912120</v>
+      </c>
+      <c r="H81" s="9">
+        <v>1596919</v>
+      </c>
+      <c r="I81" s="9">
+        <v>1674653</v>
+      </c>
+      <c r="J81" s="9">
+        <v>1645369</v>
+      </c>
+      <c r="K81" s="9">
+        <v>1852120</v>
+      </c>
+      <c r="L81" s="9">
+        <v>1607736</v>
+      </c>
+      <c r="M81" s="9">
+        <v>3393909</v>
+      </c>
+      <c r="N81" s="9">
+        <v>1740581</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B82" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11">
+        <v>0</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G82" s="11">
+        <v>51566</v>
+      </c>
+      <c r="H82" s="11">
+        <v>36604</v>
+      </c>
+      <c r="I82" s="11">
+        <v>68908</v>
+      </c>
+      <c r="J82" s="11">
+        <v>69420</v>
+      </c>
+      <c r="K82" s="11">
+        <v>25725</v>
+      </c>
+      <c r="L82" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M82" s="11">
+        <v>14359</v>
+      </c>
+      <c r="N82" s="11">
+        <v>34064</v>
+      </c>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B83" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15">
+        <v>302416</v>
+      </c>
+      <c r="F83" s="15">
+        <v>852681</v>
+      </c>
+      <c r="G83" s="15">
+        <v>1084124</v>
+      </c>
+      <c r="H83" s="15">
+        <v>1808051</v>
+      </c>
+      <c r="I83" s="15">
+        <v>1756829</v>
+      </c>
+      <c r="J83" s="15">
+        <v>1745890</v>
+      </c>
+      <c r="K83" s="15">
+        <v>2050103</v>
+      </c>
+      <c r="L83" s="15">
+        <v>2262154</v>
+      </c>
+      <c r="M83" s="15">
+        <v>3408268</v>
+      </c>
+      <c r="N83" s="15">
+        <v>3022030</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -3082,16 +3167,12 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B85" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -3101,16 +3182,12 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B86" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
@@ -3120,35 +3197,49 @@
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B87" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
-    </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
+    <row r="87" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B87" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I87" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L87" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -3158,133 +3249,2219 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B89" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F89" s="9">
+        <v>33005</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L89" s="9">
+        <v>153238</v>
+      </c>
+      <c r="M89" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N89" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B90" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11">
+        <v>91618</v>
+      </c>
+      <c r="F90" s="11">
+        <v>121325</v>
+      </c>
+      <c r="G90" s="11">
+        <v>107279</v>
+      </c>
+      <c r="H90" s="11">
+        <v>171393</v>
+      </c>
+      <c r="I90" s="11">
+        <v>61389</v>
+      </c>
+      <c r="J90" s="11">
+        <v>31101</v>
+      </c>
+      <c r="K90" s="11">
+        <v>172258</v>
+      </c>
+      <c r="L90" s="11">
+        <v>435780</v>
+      </c>
+      <c r="M90" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N90" s="11">
+        <v>1247385</v>
+      </c>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B91" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9">
+        <v>348001</v>
+      </c>
+      <c r="F91" s="9">
+        <v>484794</v>
+      </c>
+      <c r="G91" s="9">
+        <v>892514</v>
+      </c>
+      <c r="H91" s="9">
+        <v>1421653</v>
+      </c>
+      <c r="I91" s="9">
+        <v>1652078</v>
+      </c>
+      <c r="J91" s="9">
+        <v>1711412</v>
+      </c>
+      <c r="K91" s="9">
+        <v>1635142</v>
+      </c>
+      <c r="L91" s="9">
+        <v>1641653</v>
+      </c>
+      <c r="M91" s="9">
+        <v>3231215</v>
+      </c>
+      <c r="N91" s="9">
+        <v>1841019</v>
+      </c>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B92" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11">
+        <v>7081</v>
+      </c>
+      <c r="F92" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G92" s="11">
+        <v>51566</v>
+      </c>
+      <c r="H92" s="11">
+        <v>41196</v>
+      </c>
+      <c r="I92" s="11">
+        <v>42141</v>
+      </c>
+      <c r="J92" s="11">
+        <v>50109</v>
+      </c>
+      <c r="K92" s="11">
+        <v>45783</v>
+      </c>
+      <c r="L92" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M92" s="11">
+        <v>43992</v>
+      </c>
+      <c r="N92" s="11">
+        <v>55688</v>
+      </c>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B93" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" s="15"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15">
+        <v>446700</v>
+      </c>
+      <c r="F93" s="15">
+        <v>639124</v>
+      </c>
+      <c r="G93" s="15">
+        <v>1051359</v>
+      </c>
+      <c r="H93" s="15">
+        <v>1634242</v>
+      </c>
+      <c r="I93" s="15">
+        <v>1755608</v>
+      </c>
+      <c r="J93" s="15">
+        <v>1792622</v>
+      </c>
+      <c r="K93" s="15">
+        <v>1853183</v>
+      </c>
+      <c r="L93" s="15">
+        <v>2230671</v>
+      </c>
+      <c r="M93" s="15">
+        <v>3275207</v>
+      </c>
+      <c r="N93" s="15">
+        <v>3144092</v>
+      </c>
+    </row>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+    </row>
+    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+    </row>
+    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+    </row>
+    <row r="97" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B97" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J97" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K97" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L97" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M97" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N97" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+    </row>
+    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B99" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F99" s="9">
+        <v>18425</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L99" s="9">
+        <v>96317</v>
+      </c>
+      <c r="M99" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N99" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B100" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11">
+        <v>24344</v>
+      </c>
+      <c r="F100" s="11">
+        <v>31827</v>
+      </c>
+      <c r="G100" s="11">
+        <v>44986</v>
+      </c>
+      <c r="H100" s="11">
+        <v>48121</v>
+      </c>
+      <c r="I100" s="11">
+        <v>-1</v>
+      </c>
+      <c r="J100" s="11">
+        <v>0</v>
+      </c>
+      <c r="K100" s="11">
+        <v>0</v>
+      </c>
+      <c r="L100" s="11">
+        <v>0</v>
+      </c>
+      <c r="M100" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N100" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B101" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9">
+        <v>63078</v>
+      </c>
+      <c r="F101" s="9">
+        <v>286295</v>
+      </c>
+      <c r="G101" s="9">
+        <v>305901</v>
+      </c>
+      <c r="H101" s="9">
+        <v>481167</v>
+      </c>
+      <c r="I101" s="9">
+        <v>503801</v>
+      </c>
+      <c r="J101" s="9">
+        <v>437758</v>
+      </c>
+      <c r="K101" s="9">
+        <v>654736</v>
+      </c>
+      <c r="L101" s="9">
+        <v>620819</v>
+      </c>
+      <c r="M101" s="9">
+        <v>783513</v>
+      </c>
+      <c r="N101" s="9">
+        <v>683075</v>
+      </c>
+    </row>
+    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B102" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D102" s="11"/>
+      <c r="E102" s="11">
+        <v>28487</v>
+      </c>
+      <c r="F102" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" s="11">
+        <v>0</v>
+      </c>
+      <c r="H102" s="11">
+        <v>30976</v>
+      </c>
+      <c r="I102" s="11">
+        <v>57685</v>
+      </c>
+      <c r="J102" s="11">
+        <v>76995</v>
+      </c>
+      <c r="K102" s="11">
+        <v>56937</v>
+      </c>
+      <c r="L102" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M102" s="11">
+        <v>66284</v>
+      </c>
+      <c r="N102" s="11">
+        <v>45060</v>
+      </c>
+    </row>
+    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B103" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="15"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="15">
+        <v>115909</v>
+      </c>
+      <c r="F103" s="15">
+        <v>336547</v>
+      </c>
+      <c r="G103" s="15">
+        <v>350887</v>
+      </c>
+      <c r="H103" s="15">
+        <v>560264</v>
+      </c>
+      <c r="I103" s="15">
+        <v>561485</v>
+      </c>
+      <c r="J103" s="15">
+        <v>514753</v>
+      </c>
+      <c r="K103" s="15">
+        <v>711673</v>
+      </c>
+      <c r="L103" s="15">
+        <v>717136</v>
+      </c>
+      <c r="M103" s="15">
+        <v>849797</v>
+      </c>
+      <c r="N103" s="15">
+        <v>728135</v>
+      </c>
+    </row>
+    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+    </row>
+    <row r="105" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+    </row>
+    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+    </row>
+    <row r="107" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B107" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I107" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J107" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K107" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L107" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M107" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N107" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B109" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M109" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N109" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B110" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11">
+        <v>40480263</v>
+      </c>
+      <c r="F110" s="11">
+        <v>30203474</v>
+      </c>
+      <c r="G110" s="11">
+        <v>50042453</v>
+      </c>
+      <c r="H110" s="11">
+        <v>72324759</v>
+      </c>
+      <c r="I110" s="11">
+        <v>85928571</v>
+      </c>
+      <c r="J110" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K110" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L110" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M110" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N110" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B111" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9">
+        <v>31466820</v>
+      </c>
+      <c r="F111" s="9">
+        <v>17429677</v>
+      </c>
+      <c r="G111" s="9">
+        <v>45998554</v>
+      </c>
+      <c r="H111" s="9">
+        <v>50637477</v>
+      </c>
+      <c r="I111" s="9">
+        <v>78747505</v>
+      </c>
+      <c r="J111" s="9">
+        <v>76287250</v>
+      </c>
+      <c r="K111" s="9">
+        <v>86753468</v>
+      </c>
+      <c r="L111" s="9">
+        <v>105263023</v>
+      </c>
+      <c r="M111" s="9">
+        <v>124188638</v>
+      </c>
+      <c r="N111" s="9">
+        <v>158189582</v>
+      </c>
+    </row>
+    <row r="112" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B112" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L112" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M112" s="11">
+        <v>401251</v>
+      </c>
+      <c r="N112" s="11">
+        <v>370209</v>
+      </c>
+    </row>
+    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+    </row>
+    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+    </row>
+    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+    </row>
+    <row r="116" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B116" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H116" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I116" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J116" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K116" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L116" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M116" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N116" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+      <c r="N117" s="1"/>
+    </row>
+    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B118" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L118" s="9">
+        <v>914631</v>
+      </c>
+      <c r="M118" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N118" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B119" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11">
+        <v>27714474</v>
+      </c>
+      <c r="F119" s="11">
+        <v>44912134</v>
+      </c>
+      <c r="G119" s="11">
+        <v>60950405</v>
+      </c>
+      <c r="H119" s="11">
+        <v>81025070</v>
+      </c>
+      <c r="I119" s="11">
+        <v>86718954</v>
+      </c>
+      <c r="J119" s="11">
+        <v>87117647</v>
+      </c>
+      <c r="K119" s="11">
+        <v>113327632</v>
+      </c>
+      <c r="L119" s="11">
+        <v>119424500</v>
+      </c>
+      <c r="M119" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N119" s="11">
+        <v>152865809</v>
+      </c>
+    </row>
+    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B120" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9">
+        <v>20723726</v>
+      </c>
+      <c r="F120" s="9">
+        <v>39784839</v>
+      </c>
+      <c r="G120" s="9">
+        <v>50814485</v>
+      </c>
+      <c r="H120" s="9">
+        <v>71167120</v>
+      </c>
+      <c r="I120" s="9">
+        <v>77702905</v>
+      </c>
+      <c r="J120" s="9">
+        <v>82553259</v>
+      </c>
+      <c r="K120" s="9">
+        <v>99957904</v>
+      </c>
+      <c r="L120" s="9">
+        <v>110893641</v>
+      </c>
+      <c r="M120" s="9">
+        <v>151169614</v>
+      </c>
+      <c r="N120" s="9">
+        <v>143671564</v>
+      </c>
+    </row>
+    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B121" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H121" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I121" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J121" s="11">
+        <v>502</v>
+      </c>
+      <c r="K121" s="11">
+        <v>-186</v>
+      </c>
+      <c r="L121" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M121" s="11">
+        <v>410257</v>
+      </c>
+      <c r="N121" s="11">
+        <v>378489</v>
+      </c>
+    </row>
+    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
+    </row>
+    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+      <c r="N123" s="1"/>
+    </row>
+    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+      <c r="N124" s="1"/>
+    </row>
+    <row r="125" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B125" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H125" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J125" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K125" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L125" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M125" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N125" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+    </row>
+    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B127" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L127" s="9">
+        <v>641042</v>
+      </c>
+      <c r="M127" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N127" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="128" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B128" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D128" s="11"/>
+      <c r="E128" s="11">
+        <v>36098503</v>
+      </c>
+      <c r="F128" s="11">
+        <v>39935813</v>
+      </c>
+      <c r="G128" s="11">
+        <v>53909045</v>
+      </c>
+      <c r="H128" s="11">
+        <v>77308525</v>
+      </c>
+      <c r="I128" s="11">
+        <v>86099579</v>
+      </c>
+      <c r="J128" s="11">
+        <v>87117647</v>
+      </c>
+      <c r="K128" s="11">
+        <v>113327632</v>
+      </c>
+      <c r="L128" s="11">
+        <v>119424500</v>
+      </c>
+      <c r="M128" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N128" s="11">
+        <v>152865809</v>
+      </c>
+    </row>
+    <row r="129" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B129" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9">
+        <v>25340494</v>
+      </c>
+      <c r="F129" s="9">
+        <v>31913238</v>
+      </c>
+      <c r="G129" s="9">
+        <v>49220427</v>
+      </c>
+      <c r="H129" s="9">
+        <v>63557448</v>
+      </c>
+      <c r="I129" s="9">
+        <v>78449974</v>
+      </c>
+      <c r="J129" s="9">
+        <v>79641305</v>
+      </c>
+      <c r="K129" s="9">
+        <v>94217344</v>
+      </c>
+      <c r="L129" s="9">
+        <v>104437496</v>
+      </c>
+      <c r="M129" s="9">
+        <v>143628706</v>
+      </c>
+      <c r="N129" s="9">
+        <v>152895856</v>
+      </c>
+    </row>
+    <row r="130" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B130" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D130" s="11"/>
+      <c r="E130" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F130" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G130" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H130" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I130" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J130" s="11">
+        <v>543</v>
+      </c>
+      <c r="K130" s="11">
+        <v>-496</v>
+      </c>
+      <c r="L130" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M130" s="11">
+        <v>463074</v>
+      </c>
+      <c r="N130" s="11">
+        <v>362906</v>
+      </c>
+    </row>
+    <row r="131" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="K131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+      <c r="N131" s="1"/>
+    </row>
+    <row r="132" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="K132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
+    </row>
+    <row r="133" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+    </row>
+    <row r="134" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B134" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G134" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H134" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I134" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J134" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K134" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L134" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M134" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N134" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+    </row>
+    <row r="136" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B136" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L136" s="9">
+        <v>402924</v>
+      </c>
+      <c r="M136" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N136" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B137" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M137" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N137" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="138" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B138" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F138" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G138" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H138" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J138" s="9">
+        <v>86753468</v>
+      </c>
+      <c r="K138" s="9">
+        <v>105263023</v>
+      </c>
+      <c r="L138" s="9">
+        <v>124188638</v>
+      </c>
+      <c r="M138" s="9">
+        <v>158189582</v>
+      </c>
+      <c r="N138" s="9">
+        <v>135881241</v>
+      </c>
+    </row>
+    <row r="139" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B139" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C139" s="11"/>
+      <c r="D139" s="11"/>
+      <c r="E139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J139" s="11">
+        <v>1000</v>
+      </c>
+      <c r="K139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L139" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M139" s="11">
+        <v>370209</v>
+      </c>
+      <c r="N139" s="11">
+        <v>389809</v>
+      </c>
+    </row>
+    <row r="140" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="1"/>
+    </row>
+    <row r="141" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
+    </row>
+    <row r="142" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+      <c r="N142" s="1"/>
+    </row>
+    <row r="143" spans="2:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B143" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G143" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H143" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I143" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J143" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K143" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L143" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M143" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N143" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
+    </row>
+    <row r="145" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B145" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9">
+        <v>0</v>
+      </c>
+      <c r="F145" s="9">
+        <v>0</v>
+      </c>
+      <c r="G145" s="9">
+        <v>7791</v>
+      </c>
+      <c r="H145" s="9">
+        <v>-7791</v>
+      </c>
+      <c r="I145" s="9">
+        <v>7681</v>
+      </c>
+      <c r="J145" s="9">
+        <v>-7681</v>
+      </c>
+      <c r="K145" s="9">
+        <v>0</v>
+      </c>
+      <c r="L145" s="9">
+        <v>0</v>
+      </c>
+      <c r="M145" s="9">
+        <v>0</v>
+      </c>
+      <c r="N145" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B146" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C146" s="11"/>
+      <c r="D146" s="11"/>
+      <c r="E146" s="11">
+        <v>0</v>
+      </c>
+      <c r="F146" s="11">
+        <v>0</v>
+      </c>
+      <c r="G146" s="11">
+        <v>0</v>
+      </c>
+      <c r="H146" s="11">
+        <v>0</v>
+      </c>
+      <c r="I146" s="11">
+        <v>0</v>
+      </c>
+      <c r="J146" s="11">
+        <v>0</v>
+      </c>
+      <c r="K146" s="11">
+        <v>0</v>
+      </c>
+      <c r="L146" s="11">
+        <v>0</v>
+      </c>
+      <c r="M146" s="11">
+        <v>0</v>
+      </c>
+      <c r="N146" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B147" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9">
+        <v>0</v>
+      </c>
+      <c r="F147" s="9">
+        <v>0</v>
+      </c>
+      <c r="G147" s="9">
+        <v>0</v>
+      </c>
+      <c r="H147" s="9">
+        <v>0</v>
+      </c>
+      <c r="I147" s="9">
+        <v>0</v>
+      </c>
+      <c r="J147" s="9">
+        <v>0</v>
+      </c>
+      <c r="K147" s="9">
+        <v>0</v>
+      </c>
+      <c r="L147" s="9">
+        <v>0</v>
+      </c>
+      <c r="M147" s="9">
+        <v>0</v>
+      </c>
+      <c r="N147" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B148" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C148" s="11"/>
+      <c r="D148" s="11"/>
+      <c r="E148" s="11">
+        <v>0</v>
+      </c>
+      <c r="F148" s="11">
+        <v>0</v>
+      </c>
+      <c r="G148" s="11">
+        <v>0</v>
+      </c>
+      <c r="H148" s="11">
+        <v>0</v>
+      </c>
+      <c r="I148" s="11">
+        <v>1</v>
+      </c>
+      <c r="J148" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K148" s="11">
+        <v>0</v>
+      </c>
+      <c r="L148" s="11">
+        <v>0</v>
+      </c>
+      <c r="M148" s="11">
+        <v>0</v>
+      </c>
+      <c r="N148" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B149" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9">
+        <v>13421</v>
+      </c>
+      <c r="F149" s="9">
+        <v>12999</v>
+      </c>
+      <c r="G149" s="9">
+        <v>27928</v>
+      </c>
+      <c r="H149" s="9">
+        <v>25727</v>
+      </c>
+      <c r="I149" s="9">
+        <v>27158</v>
+      </c>
+      <c r="J149" s="9">
+        <v>5915</v>
+      </c>
+      <c r="K149" s="9">
+        <v>11925</v>
+      </c>
+      <c r="L149" s="9">
+        <v>36397</v>
+      </c>
+      <c r="M149" s="9">
+        <v>21411</v>
+      </c>
+      <c r="N149" s="9">
+        <v>78269</v>
+      </c>
+    </row>
+    <row r="150" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B150" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C150" s="11"/>
+      <c r="D150" s="11"/>
+      <c r="E150" s="11">
+        <v>14291</v>
+      </c>
+      <c r="F150" s="11">
+        <v>16482</v>
+      </c>
+      <c r="G150" s="11">
+        <v>-2113</v>
+      </c>
+      <c r="H150" s="11">
+        <v>34349</v>
+      </c>
+      <c r="I150" s="11">
+        <v>73</v>
+      </c>
+      <c r="J150" s="11">
+        <v>56668</v>
+      </c>
+      <c r="K150" s="11">
+        <v>42850</v>
+      </c>
+      <c r="L150" s="11">
+        <v>85798</v>
+      </c>
+      <c r="M150" s="11">
+        <v>55878</v>
+      </c>
+      <c r="N150" s="11">
+        <v>50698</v>
+      </c>
+    </row>
+    <row r="151" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B151" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="9"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
-      <c r="M89" s="1"/>
-      <c r="N89" s="1"/>
-    </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B90" s="10" t="s">
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9">
+        <v>6000</v>
+      </c>
+      <c r="F151" s="9">
+        <v>14166</v>
+      </c>
+      <c r="G151" s="9">
+        <v>-1</v>
+      </c>
+      <c r="H151" s="9">
+        <v>19271</v>
+      </c>
+      <c r="I151" s="9">
+        <v>4120</v>
+      </c>
+      <c r="J151" s="9">
+        <v>21417</v>
+      </c>
+      <c r="K151" s="9">
+        <v>16144</v>
+      </c>
+      <c r="L151" s="9">
+        <v>16807</v>
+      </c>
+      <c r="M151" s="9">
+        <v>19627</v>
+      </c>
+      <c r="N151" s="9">
+        <v>28194</v>
+      </c>
+    </row>
+    <row r="152" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B152" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C152" s="11"/>
+      <c r="D152" s="11"/>
+      <c r="E152" s="11">
+        <v>23704</v>
+      </c>
+      <c r="F152" s="11">
+        <v>54353</v>
+      </c>
+      <c r="G152" s="11">
+        <v>25152</v>
+      </c>
+      <c r="H152" s="11">
+        <v>66517</v>
+      </c>
+      <c r="I152" s="11">
+        <v>66200</v>
+      </c>
+      <c r="J152" s="11">
+        <v>57717</v>
+      </c>
+      <c r="K152" s="11">
+        <v>63151</v>
+      </c>
+      <c r="L152" s="11">
+        <v>71398</v>
+      </c>
+      <c r="M152" s="11">
+        <v>89715</v>
+      </c>
+      <c r="N152" s="11">
+        <v>112042</v>
+      </c>
+    </row>
+    <row r="153" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B153" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
-      <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B91" s="8" t="s">
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9">
+        <v>0</v>
+      </c>
+      <c r="F153" s="9">
+        <v>0</v>
+      </c>
+      <c r="G153" s="9">
+        <v>0</v>
+      </c>
+      <c r="H153" s="9">
+        <v>0</v>
+      </c>
+      <c r="I153" s="9">
+        <v>0</v>
+      </c>
+      <c r="J153" s="9">
+        <v>0</v>
+      </c>
+      <c r="K153" s="9">
+        <v>0</v>
+      </c>
+      <c r="L153" s="9">
+        <v>0</v>
+      </c>
+      <c r="M153" s="9">
+        <v>0</v>
+      </c>
+      <c r="N153" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B154" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C154" s="11"/>
+      <c r="D154" s="11"/>
+      <c r="E154" s="11">
+        <v>11124</v>
+      </c>
+      <c r="F154" s="11">
+        <v>63807</v>
+      </c>
+      <c r="G154" s="11">
+        <v>111345</v>
+      </c>
+      <c r="H154" s="11">
+        <v>4699</v>
+      </c>
+      <c r="I154" s="11">
+        <v>76241</v>
+      </c>
+      <c r="J154" s="11">
+        <v>22262</v>
+      </c>
+      <c r="K154" s="11">
+        <v>62862</v>
+      </c>
+      <c r="L154" s="11">
+        <v>85373</v>
+      </c>
+      <c r="M154" s="11">
+        <v>40060</v>
+      </c>
+      <c r="N154" s="11">
+        <v>26615</v>
+      </c>
+    </row>
+    <row r="155" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B155" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155" s="15"/>
+      <c r="D155" s="15"/>
+      <c r="E155" s="15">
+        <v>68540</v>
+      </c>
+      <c r="F155" s="15">
+        <v>161807</v>
+      </c>
+      <c r="G155" s="15">
+        <v>170102</v>
+      </c>
+      <c r="H155" s="15">
+        <v>142772</v>
+      </c>
+      <c r="I155" s="15">
+        <v>181474</v>
+      </c>
+      <c r="J155" s="15">
+        <v>156297</v>
+      </c>
+      <c r="K155" s="15">
+        <v>196932</v>
+      </c>
+      <c r="L155" s="15">
+        <v>295773</v>
+      </c>
+      <c r="M155" s="15">
+        <v>226691</v>
+      </c>
+      <c r="N155" s="15">
+        <v>295818</v>
+      </c>
+    </row>
+    <row r="156" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+    </row>
+    <row r="157" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+      <c r="N157" s="1"/>
+    </row>
+    <row r="158" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="K158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="M158" s="1"/>
+      <c r="N158" s="1"/>
+    </row>
+    <row r="159" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B159" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
-      <c r="L91" s="1"/>
-      <c r="M91" s="1"/>
-      <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" s="10" t="s">
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="K159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+      <c r="N159" s="1"/>
+    </row>
+    <row r="160" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
+    </row>
+    <row r="161" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B161" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C161" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-    </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B93" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C93" s="9" t="s">
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+      <c r="N161" s="1"/>
+    </row>
+    <row r="162" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B162" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="1"/>
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-    </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B94" s="10" t="s">
+      <c r="C162" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="D162" s="11"/>
+      <c r="E162" s="11"/>
+      <c r="F162" s="11"/>
+    </row>
+    <row r="163" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B163" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-    </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B95" s="8" t="s">
+      <c r="C163" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+    </row>
+    <row r="164" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B164" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C164" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-    </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B96" s="10" t="s">
+      <c r="D164" s="11"/>
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+    </row>
+    <row r="165" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B165" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C165" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+    </row>
+    <row r="166" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B166" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
+      <c r="C166" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D166" s="11"/>
+      <c r="E166" s="11"/>
+      <c r="F166" s="11"/>
+    </row>
+    <row r="167" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B167" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+    </row>
+    <row r="168" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B168" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D168" s="11"/>
+      <c r="E168" s="11"/>
+      <c r="F168" s="11"/>
+    </row>
+    <row r="169" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B169" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+    </row>
+    <row r="170" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B170" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C170" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D170" s="11"/>
+      <c r="E170" s="11"/>
+      <c r="F170" s="11"/>
+    </row>
+    <row r="171" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B171" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+    </row>
+    <row r="172" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B172" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C172" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D172" s="11"/>
+      <c r="E172" s="11"/>
+      <c r="F172" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>